<commit_message>
test (example): update to provide example of nested list
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouliqihan/proj/khgame/tables/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouliqihan/proj/khgame/tables/_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -114,7 +114,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>}</t>
+    <t>{</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:N14"/>
+  <dimension ref="C4:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,12 +483,19 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" customWidth="1"/>
+    <col min="16" max="16" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>7</v>
       </c>
@@ -486,19 +521,43 @@
         <v>12</v>
       </c>
       <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -520,14 +579,26 @@
       <c r="K5" t="s">
         <v>16</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>3</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>200000</v>
       </c>
@@ -540,14 +611,26 @@
       <c r="G6">
         <v>2000001</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1000001</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1000002</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>200000</v>
       </c>
@@ -560,14 +643,26 @@
       <c r="G7">
         <v>2000002</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1000001</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1000002</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>200000</v>
       </c>
@@ -580,14 +675,26 @@
       <c r="G8">
         <v>2000003</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1000001</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1000002</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>200000</v>
       </c>
@@ -600,14 +707,26 @@
       <c r="G9">
         <v>2000004</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1000001</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1000002</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>200000</v>
       </c>
@@ -620,14 +739,26 @@
       <c r="G10">
         <v>2000005</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1000001</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1000002</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>200000</v>
       </c>
@@ -640,14 +771,26 @@
       <c r="G11">
         <v>2000006</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1000001</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1000002</v>
+      </c>
+      <c r="S11">
+        <v>6</v>
+      </c>
+      <c r="T11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>200000</v>
       </c>
@@ -660,14 +803,26 @@
       <c r="G12">
         <v>2000007</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1000001</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1000002</v>
+      </c>
+      <c r="S12">
+        <v>7</v>
+      </c>
+      <c r="T12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>200000</v>
       </c>
@@ -680,14 +835,26 @@
       <c r="G13">
         <v>2000008</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>1000001</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1000002</v>
+      </c>
+      <c r="S13">
+        <v>8</v>
+      </c>
+      <c r="T13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>200000</v>
       </c>
@@ -700,11 +867,23 @@
       <c r="G14">
         <v>2000009</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>1000001</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>9</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1000002</v>
+      </c>
+      <c r="S14">
+        <v>9</v>
+      </c>
+      <c r="T14">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat (plugin): schema and convert support dynamic array
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouliqihan/proj/bagaking/starMarks_I/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouliqihan/proj/khgame/tables/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="5200" yWindow="460" windowWidth="23600" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,106 @@
   </si>
   <si>
     <t>in_town</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1|2|3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map&lt;uint&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1|2|4</t>
+  </si>
+  <si>
+    <t>tag-1</t>
+  </si>
+  <si>
+    <t>1|2|5</t>
+  </si>
+  <si>
+    <t>tag-2</t>
+  </si>
+  <si>
+    <t>1|2|6</t>
+  </si>
+  <si>
+    <t>tag-3</t>
+  </si>
+  <si>
+    <t>1|2|7</t>
+  </si>
+  <si>
+    <t>tag-4</t>
+  </si>
+  <si>
+    <t>1|2|8</t>
+  </si>
+  <si>
+    <t>tag-5</t>
+  </si>
+  <si>
+    <t>1|2|9</t>
+  </si>
+  <si>
+    <t>tag-6</t>
+  </si>
+  <si>
+    <t>1|2|10</t>
+  </si>
+  <si>
+    <t>tag-7</t>
+  </si>
+  <si>
+    <t>1|2|11</t>
+  </si>
+  <si>
+    <t>tag-8</t>
+  </si>
+  <si>
+    <t>Array&lt;float&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Dlist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -499,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R15"/>
+  <dimension ref="A2:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,15 +616,21 @@
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -535,7 +641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -546,7 +652,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -569,31 +675,61 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
         <v>14</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>17</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>11</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" t="s">
+        <v>63</v>
+      </c>
+      <c r="X5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -615,17 +751,26 @@
       <c r="J6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>15</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>3</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
@@ -641,14 +786,29 @@
       <c r="I7">
         <v>2000001</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1000001</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>2</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
@@ -664,14 +824,29 @@
       <c r="I8">
         <v>2000002</v>
       </c>
-      <c r="O8">
+      <c r="K8">
+        <v>2000001</v>
+      </c>
+      <c r="P8">
         <v>1000001</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -687,14 +862,29 @@
       <c r="I9">
         <v>2000003</v>
       </c>
-      <c r="O9">
+      <c r="K9">
+        <v>2000001</v>
+      </c>
+      <c r="P9">
         <v>1000001</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" t="s">
+        <v>47</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -710,14 +900,29 @@
       <c r="I10">
         <v>2000004</v>
       </c>
-      <c r="O10">
+      <c r="K10">
+        <v>2000001</v>
+      </c>
+      <c r="P10">
         <v>1000001</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>48</v>
+      </c>
+      <c r="U10" t="s">
+        <v>49</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>20</v>
       </c>
@@ -733,14 +938,29 @@
       <c r="I11">
         <v>2000005</v>
       </c>
-      <c r="O11">
+      <c r="K11">
+        <v>2000001</v>
+      </c>
+      <c r="P11">
         <v>1000001</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U11" t="s">
+        <v>51</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>20</v>
       </c>
@@ -756,14 +976,29 @@
       <c r="I12">
         <v>2000006</v>
       </c>
-      <c r="O12">
+      <c r="K12">
+        <v>2000001</v>
+      </c>
+      <c r="P12">
         <v>1000001</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" t="s">
+        <v>53</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>20</v>
       </c>
@@ -779,14 +1014,29 @@
       <c r="I13">
         <v>2000007</v>
       </c>
-      <c r="O13">
+      <c r="K13">
+        <v>2000001</v>
+      </c>
+      <c r="P13">
         <v>1000001</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T13" t="s">
+        <v>54</v>
+      </c>
+      <c r="U13" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>20</v>
       </c>
@@ -802,14 +1052,29 @@
       <c r="I14">
         <v>2000008</v>
       </c>
-      <c r="O14">
+      <c r="K14">
+        <v>2000001</v>
+      </c>
+      <c r="P14">
         <v>1000001</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>56</v>
+      </c>
+      <c r="U14" t="s">
+        <v>57</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>20</v>
       </c>
@@ -825,11 +1090,26 @@
       <c r="I15">
         <v>2000009</v>
       </c>
-      <c r="O15">
+      <c r="K15">
+        <v>2000001</v>
+      </c>
+      <c r="P15">
         <v>1000001</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>9</v>
+      </c>
+      <c r="T15" t="s">
+        <v>58</v>
+      </c>
+      <c r="U15" t="s">
+        <v>59</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
example: example for nest structures
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -274,7 +274,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2Dlist</t>
+    <t>nest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB15"/>
+  <dimension ref="A2:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,10 +651,12 @@
     <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="2" bestFit="1" customWidth="1"/>
     <col min="24" max="26" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -641,7 +667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -652,7 +678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -726,10 +752,25 @@
         <v>66</v>
       </c>
       <c r="AB5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -770,7 +811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
@@ -807,8 +848,11 @@
       <c r="Z7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AD7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
@@ -846,7 +890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -884,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -922,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>20</v>
       </c>
@@ -960,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>20</v>
       </c>
@@ -998,7 +1042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>20</v>
       </c>
@@ -1036,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>20</v>
       </c>
@@ -1074,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
feat (serializer): seralizer support Pair
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,7 +186,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Map&lt;uint&gt;</t>
+    <t>1|2|4</t>
+  </si>
+  <si>
+    <t>1|2|5</t>
+  </si>
+  <si>
+    <t>1|2|6</t>
+  </si>
+  <si>
+    <t>1|2|7</t>
+  </si>
+  <si>
+    <t>1|2|8</t>
+  </si>
+  <si>
+    <t>1|2|9</t>
+  </si>
+  <si>
+    <t>1|2|10</t>
+  </si>
+  <si>
+    <t>1|2|11</t>
+  </si>
+  <si>
+    <t>Array&lt;float&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair&lt;uint&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag:0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag:1</t>
+  </si>
+  <si>
+    <t>tag:2</t>
+  </si>
+  <si>
+    <t>tag:3</t>
+  </si>
+  <si>
+    <t>tag:4</t>
+  </si>
+  <si>
+    <t>tag:5</t>
+  </si>
+  <si>
+    <t>tag:6</t>
+  </si>
+  <si>
+    <t>tag:7</t>
+  </si>
+  <si>
+    <t>tag:8</t>
+  </si>
+  <si>
+    <t>pair</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -194,112 +306,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1|2|4</t>
-  </si>
-  <si>
-    <t>tag-1</t>
-  </si>
-  <si>
-    <t>1|2|5</t>
-  </si>
-  <si>
-    <t>tag-2</t>
-  </si>
-  <si>
-    <t>1|2|6</t>
-  </si>
-  <si>
-    <t>tag-3</t>
-  </si>
-  <si>
-    <t>1|2|7</t>
-  </si>
-  <si>
-    <t>tag-4</t>
-  </si>
-  <si>
-    <t>1|2|8</t>
-  </si>
-  <si>
-    <t>tag-5</t>
-  </si>
-  <si>
-    <t>1|2|9</t>
-  </si>
-  <si>
-    <t>tag-6</t>
-  </si>
-  <si>
-    <t>1|2|10</t>
-  </si>
-  <si>
-    <t>tag-7</t>
-  </si>
-  <si>
-    <t>1|2|11</t>
-  </si>
-  <si>
-    <t>tag-8</t>
-  </si>
-  <si>
-    <t>Array&lt;float&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tag-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>tag:0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array&lt;Pair&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag:s1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag:s2</t>
+  </si>
+  <si>
+    <t>tag:s3</t>
+  </si>
+  <si>
+    <t>tag:s4</t>
+  </si>
+  <si>
+    <t>tag:s5</t>
+  </si>
+  <si>
+    <t>tag:s6</t>
+  </si>
+  <si>
+    <t>tag:s7</t>
+  </si>
+  <si>
+    <t>tag:s8</t>
   </si>
 </sst>
 </file>
@@ -623,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AG15"/>
+  <dimension ref="A2:AH15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,15 +685,16 @@
     <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -667,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -678,7 +716,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -728,49 +766,52 @@
         <v>14</v>
       </c>
       <c r="T5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" t="s">
+        <v>64</v>
+      </c>
+      <c r="V5" t="s">
+        <v>77</v>
+      </c>
+      <c r="W5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" t="s">
         <v>60</v>
       </c>
-      <c r="U5" t="s">
-        <v>42</v>
-      </c>
-      <c r="V5" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="AE5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH5" t="s">
         <v>63</v>
       </c>
-      <c r="X5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -805,13 +846,16 @@
         <v>41</v>
       </c>
       <c r="U6" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="V6" t="s">
-        <v>68</v>
+        <v>75</v>
+      </c>
+      <c r="W6" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
@@ -837,22 +881,25 @@
         <v>40</v>
       </c>
       <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="X7">
+        <v>65</v>
+      </c>
+      <c r="V7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y7">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>2</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>3</v>
       </c>
-      <c r="AD7" t="s">
-        <v>73</v>
+      <c r="AE7" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
@@ -878,19 +925,22 @@
         <v>2</v>
       </c>
       <c r="T8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="U8" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8">
+        <v>66</v>
+      </c>
+      <c r="V8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y8">
         <v>1</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -916,19 +966,22 @@
         <v>3</v>
       </c>
       <c r="T9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U9" t="s">
-        <v>47</v>
-      </c>
-      <c r="X9">
+        <v>67</v>
+      </c>
+      <c r="V9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y9">
         <v>1</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -954,19 +1007,22 @@
         <v>4</v>
       </c>
       <c r="T10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="U10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X10">
+        <v>68</v>
+      </c>
+      <c r="V10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y10">
         <v>1</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>20</v>
       </c>
@@ -992,19 +1048,22 @@
         <v>5</v>
       </c>
       <c r="T11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U11" t="s">
-        <v>51</v>
-      </c>
-      <c r="X11">
+        <v>69</v>
+      </c>
+      <c r="V11" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y11">
         <v>1</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>20</v>
       </c>
@@ -1030,19 +1089,22 @@
         <v>6</v>
       </c>
       <c r="T12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="U12" t="s">
-        <v>53</v>
-      </c>
-      <c r="X12">
+        <v>70</v>
+      </c>
+      <c r="V12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y12">
         <v>1</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>20</v>
       </c>
@@ -1068,19 +1130,22 @@
         <v>7</v>
       </c>
       <c r="T13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="U13" t="s">
-        <v>55</v>
-      </c>
-      <c r="X13">
+        <v>71</v>
+      </c>
+      <c r="V13" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y13">
         <v>1</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>20</v>
       </c>
@@ -1106,19 +1171,22 @@
         <v>8</v>
       </c>
       <c r="T14" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="U14" t="s">
-        <v>57</v>
-      </c>
-      <c r="X14">
+        <v>72</v>
+      </c>
+      <c r="V14" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y14">
         <v>1</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>20</v>
       </c>
@@ -1144,15 +1212,18 @@
         <v>9</v>
       </c>
       <c r="T15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="U15" t="s">
-        <v>59</v>
-      </c>
-      <c r="X15">
+        <v>73</v>
+      </c>
+      <c r="V15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y15">
         <v>1</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doc: update logs and scripts, add examples
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,21 +147,6 @@
     <t>03</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
     <t>000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,21 +180,6 @@
     <t>1|2|6</t>
   </si>
   <si>
-    <t>1|2|7</t>
-  </si>
-  <si>
-    <t>1|2|8</t>
-  </si>
-  <si>
-    <t>1|2|9</t>
-  </si>
-  <si>
-    <t>1|2|10</t>
-  </si>
-  <si>
-    <t>1|2|11</t>
-  </si>
-  <si>
     <t>Array&lt;float&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,21 +253,6 @@
     <t>tag:3</t>
   </si>
   <si>
-    <t>tag:4</t>
-  </si>
-  <si>
-    <t>tag:5</t>
-  </si>
-  <si>
-    <t>tag:6</t>
-  </si>
-  <si>
-    <t>tag:7</t>
-  </si>
-  <si>
-    <t>tag:8</t>
-  </si>
-  <si>
     <t>pair</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,26 +279,67 @@
     <t>tag:s3</t>
   </si>
   <si>
-    <t>tag:s4</t>
-  </si>
-  <si>
-    <t>tag:s5</t>
-  </si>
-  <si>
-    <t>tag:s6</t>
-  </si>
-  <si>
-    <t>tag:s7</t>
-  </si>
-  <si>
-    <t>tag:s8</t>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair&lt;uint&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oil:388</t>
+  </si>
+  <si>
+    <t>ore1:1551</t>
+  </si>
+  <si>
+    <t>oil:416</t>
+  </si>
+  <si>
+    <t>ore1:1663</t>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair&lt;uint&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sfajdf:123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +354,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,9 +383,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -660,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AH15"/>
+  <dimension ref="A2:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AQ9" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,17 +690,23 @@
     <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -705,7 +717,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -713,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -766,57 +778,87 @@
         <v>14</v>
       </c>
       <c r="T5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="U5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="V5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="W5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="X5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="Y5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="Z5" t="s">
         <v>54</v>
       </c>
       <c r="AA5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="AB5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="AC5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="AD5" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="AE5" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="AF5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AG5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="AH5" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -843,24 +885,30 @@
         <v>4</v>
       </c>
       <c r="T6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U6" t="s">
-        <v>74</v>
-      </c>
-      <c r="V6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN6" t="s">
         <v>75</v>
       </c>
-      <c r="W6" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>26</v>
@@ -877,34 +925,44 @@
       <c r="Q7">
         <v>1</v>
       </c>
-      <c r="T7" t="s">
-        <v>40</v>
-      </c>
-      <c r="U7" t="s">
-        <v>65</v>
-      </c>
-      <c r="V7" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y7">
+      <c r="U7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="Y7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7">
         <v>1</v>
       </c>
-      <c r="Z7">
+      <c r="AE7">
         <v>2</v>
       </c>
-      <c r="AA7">
+      <c r="AF7">
         <v>3</v>
       </c>
-      <c r="AE7" t="s">
-        <v>62</v>
+      <c r="AJ7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO7">
+        <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
@@ -924,23 +982,35 @@
       <c r="Q8">
         <v>2</v>
       </c>
-      <c r="T8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U8" t="s">
-        <v>66</v>
-      </c>
-      <c r="V8" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y8">
+      <c r="U8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD8">
         <v>1</v>
       </c>
-      <c r="Z8">
+      <c r="AE8">
         <v>2</v>
       </c>
+      <c r="AO8">
+        <v>222</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -965,23 +1035,26 @@
       <c r="Q9">
         <v>3</v>
       </c>
-      <c r="T9" t="s">
-        <v>43</v>
-      </c>
-      <c r="U9" t="s">
-        <v>67</v>
-      </c>
-      <c r="V9" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y9">
+      <c r="Y9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD9">
         <v>1</v>
       </c>
-      <c r="Z9">
+      <c r="AE9">
         <v>2</v>
       </c>
+      <c r="AP9" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -1006,225 +1079,23 @@
       <c r="Q10">
         <v>4</v>
       </c>
-      <c r="T10" t="s">
-        <v>44</v>
-      </c>
-      <c r="U10" t="s">
-        <v>68</v>
-      </c>
-      <c r="V10" t="s">
+      <c r="Y10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>2</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>80</v>
-      </c>
-      <c r="Y10">
-        <v>1</v>
-      </c>
-      <c r="Z10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="D11">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>2000005</v>
-      </c>
-      <c r="K11">
-        <v>2000001</v>
-      </c>
-      <c r="P11">
-        <v>1000001</v>
-      </c>
-      <c r="Q11">
-        <v>5</v>
-      </c>
-      <c r="T11" t="s">
-        <v>45</v>
-      </c>
-      <c r="U11" t="s">
-        <v>69</v>
-      </c>
-      <c r="V11" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y11">
-        <v>1</v>
-      </c>
-      <c r="Z11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="D12">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>2000006</v>
-      </c>
-      <c r="K12">
-        <v>2000001</v>
-      </c>
-      <c r="P12">
-        <v>1000001</v>
-      </c>
-      <c r="Q12">
-        <v>6</v>
-      </c>
-      <c r="T12" t="s">
-        <v>46</v>
-      </c>
-      <c r="U12" t="s">
-        <v>70</v>
-      </c>
-      <c r="V12" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-      <c r="Z12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="D13">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>2000007</v>
-      </c>
-      <c r="K13">
-        <v>2000001</v>
-      </c>
-      <c r="P13">
-        <v>1000001</v>
-      </c>
-      <c r="Q13">
-        <v>7</v>
-      </c>
-      <c r="T13" t="s">
-        <v>47</v>
-      </c>
-      <c r="U13" t="s">
-        <v>71</v>
-      </c>
-      <c r="V13" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14">
-        <v>2000008</v>
-      </c>
-      <c r="K14">
-        <v>2000001</v>
-      </c>
-      <c r="P14">
-        <v>1000001</v>
-      </c>
-      <c r="Q14">
-        <v>8</v>
-      </c>
-      <c r="T14" t="s">
-        <v>48</v>
-      </c>
-      <c r="U14" t="s">
-        <v>72</v>
-      </c>
-      <c r="V14" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-      <c r="Z14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="D15">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <v>2000009</v>
-      </c>
-      <c r="K15">
-        <v>2000001</v>
-      </c>
-      <c r="P15">
-        <v>1000001</v>
-      </c>
-      <c r="Q15">
-        <v>9</v>
-      </c>
-      <c r="T15" t="s">
-        <v>49</v>
-      </c>
-      <c r="U15" t="s">
-        <v>73</v>
-      </c>
-      <c r="V15" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-      <c r="Z15">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat (analyze): add class Machine to handle stack
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="460" windowWidth="23600" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="5200" yWindow="460" windowWidth="23600" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -307,10 +307,6 @@
     <t>ore1:1663</t>
   </si>
   <si>
-    <t>[</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stars</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -332,6 +328,10 @@
   </si>
   <si>
     <t>sfajdf:123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oneof [</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AQ9" sqref="AQ9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +701,7 @@
     <col min="33" max="35" width="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="39" width="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="4.5" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="6" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -838,19 +839,19 @@
         <v>53</v>
       </c>
       <c r="AN5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AO5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>77</v>
       </c>
-      <c r="AP5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>78</v>
-      </c>
       <c r="AR5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
@@ -900,7 +901,7 @@
         <v>47</v>
       </c>
       <c r="AN6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
@@ -1095,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="AQ10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc: update Readme for decorators
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -331,7 +331,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>oneof [</t>
+    <t>$oneof [</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -669,7 +669,7 @@
   <dimension ref="A2:AR10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AO11" sqref="AO11"/>
+      <selection activeCell="AQ14" sqref="AQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,7 +701,7 @@
     <col min="33" max="35" width="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="39" width="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="4.5" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="6" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat (convertor): remove empty object from parent, rename typeConvertor
</commit_message>
<xml_diff>
--- a/example/nft.building.xlsx
+++ b/example/nft.building.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="460" windowWidth="23600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,6 +332,30 @@
   </si>
   <si>
     <t>$oneof [</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nestedArray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>any</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -666,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AR10"/>
+  <dimension ref="A2:AZ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AQ14" sqref="AQ14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AZ10" sqref="AZ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,9 +729,15 @@
     <col min="41" max="41" width="4.5" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="6" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -718,7 +748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -729,7 +759,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -853,8 +883,32 @@
       <c r="AR5" t="s">
         <v>75</v>
       </c>
+      <c r="AS5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -903,8 +957,17 @@
       <c r="AN6" t="s">
         <v>74</v>
       </c>
+      <c r="AS6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
@@ -957,8 +1020,11 @@
       <c r="AO7">
         <v>111</v>
       </c>
+      <c r="AU7">
+        <v>111</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
@@ -1010,8 +1076,14 @@
       <c r="AO8">
         <v>222</v>
       </c>
+      <c r="AU8">
+        <v>111</v>
+      </c>
+      <c r="AX8">
+        <v>222</v>
+      </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -1054,8 +1126,14 @@
       <c r="AP9" t="b">
         <v>1</v>
       </c>
+      <c r="AU9">
+        <v>111</v>
+      </c>
+      <c r="AX9">
+        <v>222</v>
+      </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -1097,6 +1175,12 @@
       </c>
       <c r="AQ10" t="s">
         <v>79</v>
+      </c>
+      <c r="AU10">
+        <v>111</v>
+      </c>
+      <c r="AX10">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>